<commit_message>
changed ExtractData map to use PersonInfo struct, changed testing
</commit_message>
<xml_diff>
--- a/Barringer.xlsx
+++ b/Barringer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\go\src\github.com\thatguythat1031\learnGo\CRUSMSProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C469A748-C043-489B-A30E-75EF2DD8BD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EDE5B2-C46D-4F74-9E2B-8D27DE0CCDB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="8820" windowWidth="16663" windowHeight="8863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16457" yWindow="9026" windowWidth="16457" windowHeight="8554" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8592" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8595" uniqueCount="118">
   <si>
     <t>Timestamp</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>maybe</t>
   </si>
 </sst>
 </file>
@@ -55576,10 +55582,10 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -55903,6 +55909,15 @@
       </c>
       <c r="K8" s="27" t="s">
         <v>115</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>117</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>22</v>

</xml_diff>